<commit_message>
Colorscheme of uulm added
</commit_message>
<xml_diff>
--- a/tex/colorscheme.xlsx
+++ b/tex/colorscheme.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20366"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tthuem\git\BibTags\tex\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646CE75F-8D5E-43BD-8B93-43E457BDEEAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="13605"/>
+    <workbookView xWindow="120" yWindow="48" windowWidth="24912" windowHeight="13608" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="uulm" sheetId="2" r:id="rId1"/>
+    <sheet name="ovgu" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>blue</t>
   </si>
@@ -31,12 +36,48 @@
   </si>
   <si>
     <t>gray</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>light blue</t>
+  </si>
+  <si>
+    <t>uulm</t>
+  </si>
+  <si>
+    <t>ma-wi</t>
+  </si>
+  <si>
+    <t>ing-inf</t>
+  </si>
+  <si>
+    <t>nat</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>#000000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,15 +107,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -82,14 +127,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -127,9 +175,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -162,9 +210,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,9 +262,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -372,46 +454,336 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C1" s="4">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G7" si="0">255*(1-$G$1)+C3*$G$1</f>
+        <v>178.5</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H7" si="1">255*(1-$G$1)+D3*$G$1</f>
+        <v>178.5</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I7" si="2">255*(1-$G$1)+E3*$G$1</f>
+        <v>178.5</v>
+      </c>
+      <c r="J3" t="str">
+        <f>_xlfn.CONCAT("#",DEC2HEX(G3),DEC2HEX(H3),DEC2HEX(I3))</f>
+        <v>#B2B2B2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>137</v>
+      </c>
+      <c r="D4">
+        <v>162</v>
+      </c>
+      <c r="E4">
+        <v>179</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT("#",DEC2HEX(C4),DEC2HEX(D4),DEC2HEX(E4))</f>
+        <v>#89A2B3</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>219.6</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="1"/>
+        <v>227.1</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="2"/>
+        <v>232.2</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J8" si="3">_xlfn.CONCAT("#",DEC2HEX(G4),DEC2HEX(H4),DEC2HEX(I4))</f>
+        <v>#DBE3E8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>86</v>
+      </c>
+      <c r="D5">
+        <v>170</v>
+      </c>
+      <c r="E5">
+        <v>28</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F8" si="4">_xlfn.CONCAT("#",DEC2HEX(C5),DEC2HEX(D5),DEC2HEX(E5))</f>
+        <v>#56AA1C</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>204.3</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>229.5</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="2"/>
+        <v>186.9</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="3"/>
+        <v>#CCE5BA</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>136</v>
+      </c>
+      <c r="D6">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <v>56</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="4"/>
+        <v>#882638</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>219.3</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>189.9</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="2"/>
+        <v>195.3</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="3"/>
+        <v>#DBBDC3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>223</v>
+      </c>
+      <c r="D7">
+        <v>109</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7" t="str">
+        <f>_xlfn.CONCAT("#",DEC2HEX(C7),DEC2HEX(D7),"0",DEC2HEX(E7))</f>
+        <v>#DF6D07</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>245.39999999999998</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>211.2</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="2"/>
+        <v>180.6</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="3"/>
+        <v>#F5D3B4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>84</v>
+      </c>
+      <c r="E8">
+        <v>124</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="4"/>
+        <v>#26547C</v>
+      </c>
+      <c r="G8" s="1">
+        <f>255*(1-$G$1)+C8*$G$1</f>
+        <v>189.9</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" ref="H8:I8" si="5">255*(1-$G$1)+D8*$G$1</f>
+        <v>203.7</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="5"/>
+        <v>215.7</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="3"/>
+        <v>#BDCBD7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
       <c r="M1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -448,12 +820,12 @@
       <c r="L2">
         <v>6</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <f>AVERAGE(A2:L2)</f>
         <v>97.416666666666671</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>40</v>
       </c>
@@ -490,12 +862,12 @@
       <c r="L3">
         <v>59</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <f t="shared" ref="M3:M6" si="0">AVERAGE(A3:L3)</f>
         <v>93.75</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -532,12 +904,12 @@
       <c r="L4">
         <v>3</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <f t="shared" si="0"/>
         <v>52.5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>76</v>
       </c>
@@ -574,12 +946,12 @@
       <c r="L5">
         <v>88</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <f t="shared" si="0"/>
         <v>152.25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>136</v>
       </c>
@@ -616,7 +988,7 @@
       <c r="L6">
         <v>154</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="1">
         <f t="shared" si="0"/>
         <v>188.66666666666666</v>
       </c>
@@ -631,28 +1003,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>